<commit_message>
ADDED REFERENCES FOR COMPONENTS ON SCHEMATIC
</commit_message>
<xml_diff>
--- a/docs/subfolder/BillofMaterials.xlsx
+++ b/docs/subfolder/BillofMaterials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LuisA\Documents\Github Files\luisAsaenz.github.io\luisAsaenz.github.io\docs\subfolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD7F540-1B79-4343-96FA-0C40989D29D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45090222-EE7C-4299-BFA1-8ACCED73B7A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10178" yWindow="0" windowWidth="10425" windowHeight="13043" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="157">
   <si>
     <t>Bill of Materials Example</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Schematic Reference Designators</t>
   </si>
   <si>
-    <t>U1</t>
-  </si>
-  <si>
     <t>Test points</t>
   </si>
   <si>
@@ -441,6 +438,72 @@
   </si>
   <si>
     <t>1727-7840-1-ND</t>
+  </si>
+  <si>
+    <t>SW1, SW2</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R4,R1</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>C10,C11</t>
+  </si>
+  <si>
+    <t>J7,J6</t>
+  </si>
+  <si>
+    <t>D4,D5</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>U4,U5,U6,U7</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C9,C8,C7,C3</t>
+  </si>
+  <si>
+    <t>J10,J8,J3</t>
+  </si>
+  <si>
+    <t>U2</t>
   </si>
 </sst>
 </file>
@@ -450,7 +513,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -486,6 +549,10 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -892,8 +959,8 @@
   </sheetPr>
   <dimension ref="A1:Q101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="68" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -991,7 +1058,7 @@
     </row>
     <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="3">
         <v>3</v>
@@ -1011,22 +1078,22 @@
         <v>1.3800000000000001</v>
       </c>
       <c r="G3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="I3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="9" t="s">
+      <c r="K3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>29</v>
       </c>
       <c r="M3" s="2">
         <v>0</v>
@@ -1040,12 +1107,12 @@
         <v>-3</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>18</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" s="3">
         <v>4</v>
@@ -1065,22 +1132,22 @@
         <v>0.33600000000000002</v>
       </c>
       <c r="G4" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="I4" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="J4" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="J4" s="7" t="s">
-        <v>88</v>
-      </c>
       <c r="K4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M4" s="2">
         <v>0</v>
@@ -1093,11 +1160,13 @@
         <f t="shared" si="2"/>
         <v>-4</v>
       </c>
-      <c r="Q4" s="2"/>
+      <c r="Q4" s="2" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" s="3">
         <v>3</v>
@@ -1117,22 +1186,22 @@
         <v>6.09</v>
       </c>
       <c r="G5" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="I5" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="J5" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="K5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="K5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>100</v>
       </c>
       <c r="M5" s="2">
         <v>0</v>
@@ -1145,11 +1214,13 @@
         <f t="shared" si="2"/>
         <v>-3</v>
       </c>
-      <c r="Q5" s="2"/>
+      <c r="Q5" s="2" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
@@ -1169,22 +1240,22 @@
         <v>8.36</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H6" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="I6" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="J6" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="K6" t="s">
+        <v>29</v>
+      </c>
+      <c r="L6" s="7" t="s">
         <v>110</v>
-      </c>
-      <c r="K6" t="s">
-        <v>30</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>111</v>
       </c>
       <c r="M6" s="2">
         <v>0</v>
@@ -1197,11 +1268,13 @@
         <f t="shared" si="2"/>
         <v>-2</v>
       </c>
-      <c r="Q6" s="2"/>
+      <c r="Q6" s="2" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B7" s="3">
         <v>2</v>
@@ -1221,22 +1294,22 @@
         <v>10.38</v>
       </c>
       <c r="G7" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="H7" s="7" t="s">
-        <v>116</v>
-      </c>
       <c r="I7" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="J7" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="K7" t="s">
+        <v>29</v>
+      </c>
+      <c r="L7" s="7" t="s">
         <v>113</v>
-      </c>
-      <c r="K7" t="s">
-        <v>30</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>114</v>
       </c>
       <c r="M7" s="2">
         <v>0</v>
@@ -1249,11 +1322,13 @@
         <f t="shared" si="2"/>
         <v>-2</v>
       </c>
-      <c r="Q7" s="2"/>
+      <c r="Q7" s="2" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B8" s="3">
         <v>4</v>
@@ -1273,22 +1348,22 @@
         <v>0.44</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H8" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="K8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L8" s="7" t="s">
         <v>91</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="K8" t="s">
-        <v>30</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>92</v>
       </c>
       <c r="M8" s="2">
         <v>0</v>
@@ -1301,11 +1376,13 @@
         <f t="shared" si="2"/>
         <v>-4</v>
       </c>
-      <c r="Q8" s="2"/>
+      <c r="Q8" s="2" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B9" s="3">
         <v>4</v>
@@ -1325,22 +1402,22 @@
         <v>0.52</v>
       </c>
       <c r="G9" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="J9" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="H9" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="I9" s="7" t="s">
+      <c r="K9" t="s">
+        <v>29</v>
+      </c>
+      <c r="L9" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="K9" t="s">
-        <v>30</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>106</v>
       </c>
       <c r="M9" s="2">
         <v>0</v>
@@ -1353,11 +1430,13 @@
         <f t="shared" si="2"/>
         <v>-4</v>
       </c>
-      <c r="Q9" s="2"/>
+      <c r="Q9" s="2" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="10" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B10" s="3">
         <v>3</v>
@@ -1377,22 +1456,22 @@
         <v>0.81</v>
       </c>
       <c r="G10" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="J10" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="H10" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>81</v>
-      </c>
       <c r="K10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M10" s="2">
         <v>0</v>
@@ -1405,10 +1484,13 @@
         <f t="shared" si="2"/>
         <v>-3</v>
       </c>
+      <c r="Q10" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B11" s="3">
         <v>3</v>
@@ -1428,22 +1510,22 @@
         <v>1.32</v>
       </c>
       <c r="G11" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="H11" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="I11" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="J11" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="J11" s="9" t="s">
+      <c r="K11" t="s">
+        <v>29</v>
+      </c>
+      <c r="L11" s="8" t="s">
         <v>122</v>
-      </c>
-      <c r="K11" t="s">
-        <v>30</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>123</v>
       </c>
       <c r="M11" s="2">
         <v>0</v>
@@ -1456,10 +1538,13 @@
         <f t="shared" si="2"/>
         <v>-3</v>
       </c>
+      <c r="Q11" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B12" s="3">
         <v>3</v>
@@ -1479,22 +1564,22 @@
         <v>0.96</v>
       </c>
       <c r="G12" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I12" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="H12" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="I12" s="8" t="s">
+      <c r="J12" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="K12" t="s">
+        <v>29</v>
+      </c>
+      <c r="L12" s="8" t="s">
         <v>68</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="K12" t="s">
-        <v>30</v>
-      </c>
-      <c r="L12" s="8" t="s">
-        <v>69</v>
       </c>
       <c r="M12" s="2">
         <v>0</v>
@@ -1507,10 +1592,13 @@
         <f t="shared" si="2"/>
         <v>-3</v>
       </c>
+      <c r="Q12" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="13" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" s="3">
         <v>2</v>
@@ -1530,22 +1618,22 @@
         <v>1.54</v>
       </c>
       <c r="G13" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I13" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="I13" s="8" t="s">
+      <c r="J13" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="J13" s="8" t="s">
-        <v>49</v>
-      </c>
       <c r="K13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M13" s="2">
         <v>0</v>
@@ -1558,10 +1646,13 @@
         <f t="shared" si="2"/>
         <v>-2</v>
       </c>
+      <c r="Q13" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="3">
         <v>2</v>
@@ -1581,22 +1672,22 @@
         <v>2.1</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="J14" s="8" t="s">
-        <v>35</v>
-      </c>
       <c r="K14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M14" s="2">
         <v>0</v>
@@ -1609,10 +1700,13 @@
         <f t="shared" si="2"/>
         <v>-2</v>
       </c>
+      <c r="Q14" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="15" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" s="3">
         <v>2</v>
@@ -1632,22 +1726,22 @@
         <v>10.119999999999999</v>
       </c>
       <c r="G15" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H15" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="I15" s="8" t="s">
+      <c r="J15" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="J15" s="8" t="s">
-        <v>42</v>
-      </c>
       <c r="K15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M15" s="2">
         <v>0</v>
@@ -1660,10 +1754,13 @@
         <f t="shared" si="2"/>
         <v>-2</v>
       </c>
+      <c r="Q15" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="16" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16" s="3">
         <v>2</v>
@@ -1683,22 +1780,22 @@
         <v>6.64</v>
       </c>
       <c r="G16" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="I16" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="J16" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="K16" t="s">
+        <v>29</v>
+      </c>
+      <c r="L16" s="8" t="s">
         <v>54</v>
-      </c>
-      <c r="K16" t="s">
-        <v>30</v>
-      </c>
-      <c r="L16" s="8" t="s">
-        <v>55</v>
       </c>
       <c r="M16" s="2">
         <v>0</v>
@@ -1711,10 +1808,13 @@
         <f t="shared" si="2"/>
         <v>-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" s="3">
         <v>10</v>
@@ -1734,22 +1834,22 @@
         <v>2.1</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H17" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="K17" t="s">
+        <v>29</v>
+      </c>
+      <c r="L17" s="8" t="s">
         <v>64</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="K17" t="s">
-        <v>30</v>
-      </c>
-      <c r="L17" s="8" t="s">
-        <v>65</v>
       </c>
       <c r="M17" s="2">
         <v>0</v>
@@ -1762,10 +1862,13 @@
         <f>O17-B17</f>
         <v>-10</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q17" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B18" s="3">
         <v>4</v>
@@ -1785,22 +1888,22 @@
         <v>0.72</v>
       </c>
       <c r="G18" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="I18" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="K18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L18" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="J18" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="K18" t="s">
-        <v>30</v>
-      </c>
-      <c r="L18" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="M18" s="2">
         <v>0</v>
@@ -1813,10 +1916,13 @@
         <f t="shared" si="2"/>
         <v>-4</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q18" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="3">
         <v>4</v>
@@ -1836,22 +1942,22 @@
         <v>3.8</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H19" s="8">
         <v>702460801</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M19" s="2">
         <v>0</v>
@@ -1864,10 +1970,13 @@
         <f t="shared" si="2"/>
         <v>-4</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q19" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B20" s="3">
         <v>2</v>
@@ -1887,22 +1996,22 @@
         <v>2.02</v>
       </c>
       <c r="G20" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H20" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="H20" s="8" t="s">
+      <c r="I20" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="I20" s="8" t="s">
+      <c r="J20" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="J20" s="8" t="s">
+      <c r="K20" t="s">
+        <v>29</v>
+      </c>
+      <c r="L20" s="8" t="s">
         <v>75</v>
-      </c>
-      <c r="K20" t="s">
-        <v>30</v>
-      </c>
-      <c r="L20" s="8" t="s">
-        <v>76</v>
       </c>
       <c r="M20" s="2">
         <v>0</v>
@@ -1915,10 +2024,13 @@
         <f>O20-B20</f>
         <v>-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q20" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B21" s="3">
         <v>10</v>
@@ -1938,22 +2050,22 @@
         <v>0.49</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H21" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="I21" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="J21" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="J21" s="8" t="s">
+      <c r="K21" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L21" s="8" t="s">
         <v>128</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="L21" s="8" t="s">
-        <v>129</v>
       </c>
       <c r="M21" s="2">
         <v>0</v>
@@ -1965,10 +2077,13 @@
         <f>O21-B21</f>
         <v>-10</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q21" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B22" s="3">
         <v>10</v>
@@ -1988,22 +2103,22 @@
         <v>1.18</v>
       </c>
       <c r="G22" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="I22" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="H22" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="I22" s="9" t="s">
+      <c r="J22" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="J22" s="8" t="s">
+      <c r="K22" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L22" s="8" t="s">
         <v>134</v>
-      </c>
-      <c r="K22" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="L22" s="8" t="s">
-        <v>135</v>
       </c>
       <c r="M22" s="2">
         <v>0</v>
@@ -2015,10 +2130,13 @@
         <f>O22-B22</f>
         <v>-10</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q22" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="3">
         <v>8</v>
@@ -2038,7 +2156,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M23" s="2">
         <v>0</v>
@@ -2051,10 +2169,13 @@
         <f>O23-B23</f>
         <v>-8</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q23" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="3">
         <v>3</v>
@@ -2074,7 +2195,7 @@
         <v>0</v>
       </c>
       <c r="K24" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M24" s="2">
         <v>0</v>
@@ -2087,8 +2208,11 @@
         <f>O24-B24</f>
         <v>-3</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q24" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="3"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4">
@@ -2106,7 +2230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="3"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4">
@@ -2124,7 +2248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="3"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4">
@@ -2142,7 +2266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="3"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4">
@@ -2160,7 +2284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B29" s="3"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4">
@@ -2178,7 +2302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B30" s="3"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4">
@@ -2196,7 +2320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B31" s="3"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4">
@@ -2214,7 +2338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B32" s="3"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4">
@@ -3478,6 +3602,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:Q1"/>
   </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="J3" r:id="rId1" xr:uid="{8E1E49D0-1F3D-4F0E-A2D0-E4E416E480D3}"/>
     <hyperlink ref="I3" r:id="rId2" xr:uid="{CB90F7FD-E2CB-48BF-AB4F-80D1BD13579F}"/>

</xml_diff>

<commit_message>
updated Bill of Materials with additional components and corrected references
</commit_message>
<xml_diff>
--- a/docs/subfolder/BillofMaterials.xlsx
+++ b/docs/subfolder/BillofMaterials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LuisA\Documents\Github Files\luisAsaenz.github.io\luisAsaenz.github.io\docs\subfolder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3f2e35d8c5d1661c/Desktop/Github Websites/luisAsaenz.github.io/docs/subfolder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45090222-EE7C-4299-BFA1-8ACCED73B7A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{45090222-EE7C-4299-BFA1-8ACCED73B7A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{654C1A81-456E-4EAA-9BC5-D6489865600B}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="164">
   <si>
     <t>Bill of Materials Example</t>
   </si>
@@ -476,9 +476,6 @@
     <t>J7,J6</t>
   </si>
   <si>
-    <t>D4,D5</t>
-  </si>
-  <si>
     <t>R3</t>
   </si>
   <si>
@@ -504,6 +501,30 @@
   </si>
   <si>
     <t>U2</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 20V 1A TUMD2M</t>
+  </si>
+  <si>
+    <t>Rohm Semiconductor</t>
+  </si>
+  <si>
+    <t>RB161VAM-20TR</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/rohm-semiconductor/RB161VAM-20TR/5955698</t>
+  </si>
+  <si>
+    <t>https://www.rohm.com/datasheet?p=RB161VAM-20&amp;dist=Digi-key&amp;media=referral&amp;source=digi-key.com&amp;campaign=Digi-key</t>
+  </si>
+  <si>
+    <t>RB161VAM-20CT-ND</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D6,D5</t>
   </si>
 </sst>
 </file>
@@ -960,7 +981,7 @@
   <dimension ref="A1:Q101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="68" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1161,7 +1182,7 @@
         <v>-4</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1215,7 +1236,7 @@
         <v>-3</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1269,7 +1290,7 @@
         <v>-2</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1431,7 +1452,7 @@
         <v>-4</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1755,7 +1776,7 @@
         <v>-2</v>
       </c>
       <c r="Q15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1809,7 +1830,7 @@
         <v>-2</v>
       </c>
       <c r="Q16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1917,7 +1938,7 @@
         <v>-4</v>
       </c>
       <c r="Q18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2131,7 +2152,7 @@
         <v>-10</v>
       </c>
       <c r="Q22" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2170,7 +2191,7 @@
         <v>-8</v>
       </c>
       <c r="Q23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2209,25 +2230,55 @@
         <v>-3</v>
       </c>
       <c r="Q24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="3"/>
-      <c r="C25" s="4"/>
+      <c r="A25" t="s">
+        <v>156</v>
+      </c>
+      <c r="B25" s="3">
+        <v>3</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0.43</v>
+      </c>
       <c r="D25" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E25" s="4"/>
+        <v>1.29</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0.43</v>
+      </c>
       <c r="F25" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.29</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="K25" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L25" s="8" t="s">
+        <v>161</v>
       </c>
       <c r="N25" s="5"/>
       <c r="P25" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-3</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="26" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3609,6 +3660,7 @@
     <hyperlink ref="J11" r:id="rId3" xr:uid="{3FBA74AE-EAF5-4D30-A7BA-7FFE1DE0334B}"/>
     <hyperlink ref="I18" r:id="rId4" xr:uid="{96B640F6-26D6-4741-A0A3-99D2BFF08648}"/>
     <hyperlink ref="I22" r:id="rId5" xr:uid="{CF4FCBC2-B8D9-4E1C-BE68-F356981257FA}"/>
+    <hyperlink ref="I25" r:id="rId6" xr:uid="{0F5D428F-9863-41BF-AACA-51F49FBE013D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>